<commit_message>
creating files for power bi version
</commit_message>
<xml_diff>
--- a/Excel/Sales_Performance_Data.xlsx
+++ b/Excel/Sales_Performance_Data.xlsx
@@ -5,17 +5,16 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sales_performance_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sales-Performance-Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CFE19-3080-46CF-A538-7685CFC57AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2E3C68-F2EB-48D0-9EB4-038CE5AD6E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="working sheet" sheetId="1" r:id="rId1"/>
     <sheet name="dashboard" sheetId="2" r:id="rId2"/>
-    <sheet name="insights" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Product">#N/A</definedName>
@@ -24,14 +23,14 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
+        <x14:slicerCache r:id="rId4"/>
         <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
-        <x14:slicerCache r:id="rId7"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -4728,7 +4727,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>154775</xdr:rowOff>
@@ -4765,13 +4764,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>159541</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>11907</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>145254</xdr:rowOff>
     </xdr:to>
@@ -4800,8 +4799,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>169071</xdr:rowOff>
     </xdr:from>
@@ -4837,13 +4836,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>2380</xdr:colOff>
+      <xdr:colOff>2381</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>159545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>11907</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>164308</xdr:rowOff>
     </xdr:to>
@@ -4872,19 +4871,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>166689</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>631031</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>176214</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="8" name="Product">
@@ -4907,7 +4906,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4917,7 +4916,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="19619799" y="411618"/>
+              <a:off x="18347531" y="404814"/>
               <a:ext cx="1821656" cy="1724025"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4950,19 +4949,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>30957</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>411957</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="Region">
@@ -4985,7 +4984,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4995,7 +4994,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="19626944" y="3302454"/>
+              <a:off x="18354676" y="3295650"/>
               <a:ext cx="1821656" cy="1447800"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5028,19 +5027,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>11906</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>109538</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>631031</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="Year">
@@ -5063,7 +5062,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -5073,7 +5072,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="19619799" y="2259467"/>
+              <a:off x="18347531" y="2252663"/>
               <a:ext cx="1821656" cy="962025"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11191,310 +11190,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8F14F47-FA7D-4709-86F8-54F0919245CA}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Sales Rep">
-  <location ref="A38:B44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="6">
-        <item x="4"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total Sales" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{07DDD4D0-033D-44E0-B8BE-258DF27F99B2}" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Region">
-  <location ref="A30:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total Sales" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09F7866E-4776-46FF-BDEE-B48726E8C057}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Product">
-  <location ref="A20:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="6">
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total Sales" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1470C31-068A-4C62-9386-4F96A3559427}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Month" colHeaderCaption="Year">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1470C31-068A-4C62-9386-4F96A3559427}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Month" colHeaderCaption="Year">
   <location ref="A1:D15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -11629,6 +11325,309 @@
           </reference>
           <reference field="9" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8F14F47-FA7D-4709-86F8-54F0919245CA}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Sales Rep">
+  <location ref="A38:B44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="6">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total Sales" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{07DDD4D0-033D-44E0-B8BE-258DF27F99B2}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Region">
+  <location ref="A30:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total Sales" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09F7866E-4776-46FF-BDEE-B48726E8C057}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Product">
+  <location ref="A20:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="6">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total Sales" fld="7" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -29090,7 +29089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB86DC9-F87E-41CF-B7DD-BB6C31E53CF4}">
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
@@ -29523,16 +29522,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3599F77-7A03-431E-B01A-E2F4FF952610}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>